<commit_message>
整理文件 Signed-off-by: anshu.wang.work@gmail.com <anshu.wang.work@gmail.com>
</commit_message>
<xml_diff>
--- a/分享内容/插件实现过程/插件实现过程.xlsx
+++ b/分享内容/插件实现过程/插件实现过程.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21600" windowHeight="10800" tabRatio="886" firstSheet="1" activeTab="11"/>
+    <workbookView windowWidth="22943" windowHeight="9804" tabRatio="886" firstSheet="1" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="应用文体综述型文章" sheetId="6" r:id="rId1"/>
@@ -1542,16 +1542,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ \￥* #,##0.00_ ;_ \￥* \-#,##0.00_ ;_ \￥* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ \￥* #,##0_ ;_ \￥* \-#,##0_ ;_ \￥* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="35">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -1559,7 +1559,7 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -1567,7 +1567,7 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -1580,7 +1580,7 @@
     <font>
       <sz val="9"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -1593,7 +1593,7 @@
     <font>
       <sz val="11"/>
       <color theme="0" tint="-0.05"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -1601,7 +1601,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -1609,7 +1609,7 @@
       <u/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -1629,16 +1629,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -1646,14 +1652,38 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -1661,7 +1691,29 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -1669,81 +1721,14 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -1751,7 +1736,22 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -1827,7 +1827,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1839,19 +1935,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1863,13 +1977,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1881,133 +2001,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2183,41 +2183,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2237,22 +2207,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2280,153 +2260,173 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="17" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2541,55 +2541,55 @@
     </xf>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -2637,8 +2637,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4324350" y="620395"/>
-          <a:ext cx="4037330" cy="352425"/>
+          <a:off x="3912870" y="654685"/>
+          <a:ext cx="3634105" cy="375285"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2679,8 +2679,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="635" y="333375"/>
-          <a:ext cx="2276475" cy="4380865"/>
+          <a:off x="635" y="344805"/>
+          <a:ext cx="2070735" cy="4678045"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2721,8 +2721,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="238125" y="1790700"/>
-          <a:ext cx="1162050" cy="247650"/>
+          <a:off x="238125" y="1905000"/>
+          <a:ext cx="1024890" cy="259080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2763,8 +2763,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1270" y="3943350"/>
-          <a:ext cx="1284605" cy="238125"/>
+          <a:off x="1270" y="4206240"/>
+          <a:ext cx="1216025" cy="249555"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2805,8 +2805,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1085850" y="4229100"/>
-          <a:ext cx="1133475" cy="209550"/>
+          <a:off x="1017270" y="4503420"/>
+          <a:ext cx="996315" cy="220980"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2839,8 +2839,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="12774295" y="1933575"/>
-          <a:ext cx="1789430" cy="1732915"/>
+          <a:off x="11508740" y="2059305"/>
+          <a:ext cx="1652270" cy="1847215"/>
           <a:chOff x="17385" y="3030"/>
           <a:chExt cx="2818" cy="3284"/>
         </a:xfrm>
@@ -2946,8 +2946,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="12812395" y="6915150"/>
-          <a:ext cx="1424305" cy="552450"/>
+          <a:off x="11546840" y="7372350"/>
+          <a:ext cx="1287145" cy="586740"/>
           <a:chOff x="20355" y="7170"/>
           <a:chExt cx="2243" cy="870"/>
         </a:xfrm>
@@ -3053,8 +3053,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="12850495" y="4504055"/>
-          <a:ext cx="1443355" cy="1418590"/>
+          <a:off x="11584940" y="4801235"/>
+          <a:ext cx="1306195" cy="1510030"/>
           <a:chOff x="20610" y="7558"/>
           <a:chExt cx="2273" cy="2234"/>
         </a:xfrm>
@@ -3172,8 +3172,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5486400" y="2228850"/>
-          <a:ext cx="304800" cy="304800"/>
+          <a:off x="4937760" y="2377440"/>
+          <a:ext cx="304800" cy="316230"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3206,8 +3206,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="227965" y="1543050"/>
-          <a:ext cx="9782810" cy="5925820"/>
+          <a:off x="227965" y="1645920"/>
+          <a:ext cx="8822690" cy="6314440"/>
           <a:chOff x="6389" y="3075"/>
           <a:chExt cx="13516" cy="10352"/>
         </a:xfrm>
@@ -5917,8 +5917,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="2626360" y="287655"/>
-          <a:ext cx="678815" cy="4391660"/>
+          <a:off x="2329180" y="653415"/>
+          <a:ext cx="724535" cy="3980180"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -5966,8 +5966,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000" flipV="1">
-          <a:off x="669290" y="3510280"/>
-          <a:ext cx="203835" cy="635"/>
+          <a:off x="589280" y="3738880"/>
+          <a:ext cx="226695" cy="635"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -6015,8 +6015,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="670560" y="4314825"/>
-          <a:ext cx="201295" cy="635"/>
+          <a:off x="596265" y="4594860"/>
+          <a:ext cx="212725" cy="635"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -6064,8 +6064,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="654685" y="5131435"/>
-          <a:ext cx="229870" cy="3175"/>
+          <a:off x="580390" y="5468620"/>
+          <a:ext cx="241300" cy="3175"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -6111,8 +6111,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2395855" y="3408680"/>
-          <a:ext cx="0" cy="179705"/>
+          <a:off x="2190115" y="3625850"/>
+          <a:ext cx="0" cy="191135"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -6158,8 +6158,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="2288540" y="4279265"/>
-          <a:ext cx="215265" cy="3175"/>
+          <a:off x="2077085" y="4559300"/>
+          <a:ext cx="226695" cy="3175"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -6205,8 +6205,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="2282190" y="5099685"/>
-          <a:ext cx="224790" cy="3175"/>
+          <a:off x="2070735" y="5436870"/>
+          <a:ext cx="236220" cy="3175"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -6234,7 +6234,7 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>336232</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>177482</xdr:rowOff>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
@@ -6252,8 +6252,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="2289175" y="5933440"/>
-          <a:ext cx="211455" cy="3175"/>
+          <a:off x="2072005" y="6322060"/>
+          <a:ext cx="234315" cy="3175"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -6299,8 +6299,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="2291715" y="6762750"/>
-          <a:ext cx="205740" cy="3175"/>
+          <a:off x="2074545" y="7208520"/>
+          <a:ext cx="228600" cy="3175"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -6346,8 +6346,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="3723640" y="3499485"/>
-          <a:ext cx="180975" cy="3175"/>
+          <a:off x="3375025" y="3722370"/>
+          <a:ext cx="192405" cy="3175"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -6393,8 +6393,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000" flipV="1">
-          <a:off x="3658870" y="4291965"/>
-          <a:ext cx="310515" cy="635"/>
+          <a:off x="3310255" y="4572000"/>
+          <a:ext cx="321945" cy="635"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -6442,8 +6442,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="3688715" y="5121910"/>
-          <a:ext cx="252095" cy="3175"/>
+          <a:off x="3340100" y="5459095"/>
+          <a:ext cx="263525" cy="3175"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -6489,8 +6489,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000">
-          <a:off x="4148455" y="1810385"/>
-          <a:ext cx="679450" cy="1348740"/>
+          <a:off x="3714115" y="2038985"/>
+          <a:ext cx="725170" cy="1211580"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -6538,8 +6538,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000">
-          <a:off x="4766945" y="2437765"/>
-          <a:ext cx="688340" cy="100965"/>
+          <a:off x="4264025" y="2597785"/>
+          <a:ext cx="734060" cy="100965"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -6587,8 +6587,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipV="1">
-          <a:off x="5521960" y="1785620"/>
-          <a:ext cx="664845" cy="1383665"/>
+          <a:off x="4950460" y="2014220"/>
+          <a:ext cx="710565" cy="1246505"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -6636,8 +6636,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipV="1">
-          <a:off x="6250940" y="1054735"/>
-          <a:ext cx="674370" cy="2853055"/>
+          <a:off x="5610860" y="1351915"/>
+          <a:ext cx="720090" cy="2578735"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -6685,8 +6685,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipV="1">
-          <a:off x="6968490" y="339090"/>
-          <a:ext cx="693420" cy="4305300"/>
+          <a:off x="6259830" y="704850"/>
+          <a:ext cx="739140" cy="3893820"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -6734,8 +6734,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000">
-          <a:off x="3439795" y="1101090"/>
-          <a:ext cx="678815" cy="2766695"/>
+          <a:off x="3074035" y="1398270"/>
+          <a:ext cx="724535" cy="2492375"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -6780,8 +6780,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="10085070" y="1390650"/>
-          <a:ext cx="19592925" cy="14630400"/>
+          <a:off x="9124950" y="1482090"/>
+          <a:ext cx="17604105" cy="15601950"/>
           <a:chOff x="1512" y="9585"/>
           <a:chExt cx="26940" cy="25590"/>
         </a:xfrm>
@@ -6892,7 +6892,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="635" y="635"/>
-          <a:ext cx="5824855" cy="5299710"/>
+          <a:ext cx="5276215" cy="5642610"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6926,8 +6926,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2762250" y="3629025"/>
-          <a:ext cx="6972300" cy="342900"/>
+          <a:off x="2487930" y="3869055"/>
+          <a:ext cx="6286500" cy="365760"/>
         </a:xfrm>
         <a:prstGeom prst="cube">
           <a:avLst/>
@@ -6991,8 +6991,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2781300" y="3152775"/>
-          <a:ext cx="6962775" cy="428625"/>
+          <a:off x="2506980" y="3358515"/>
+          <a:ext cx="6276975" cy="451485"/>
           <a:chOff x="4365" y="4650"/>
           <a:chExt cx="10965" cy="675"/>
         </a:xfrm>
@@ -7485,8 +7485,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="800100" y="4800600"/>
-          <a:ext cx="1171575" cy="1038225"/>
+          <a:off x="731520" y="5120640"/>
+          <a:ext cx="1102995" cy="1106805"/>
         </a:xfrm>
         <a:prstGeom prst="cube">
           <a:avLst/>
@@ -7554,8 +7554,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4905375" y="4619625"/>
-          <a:ext cx="1866900" cy="1828800"/>
+          <a:off x="4425315" y="4916805"/>
+          <a:ext cx="1729740" cy="1954530"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartAlternateProcess">
           <a:avLst/>
@@ -7615,8 +7615,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5267325" y="4305300"/>
-          <a:ext cx="1181100" cy="419100"/>
+          <a:off x="4787265" y="4591050"/>
+          <a:ext cx="1043940" cy="441960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7672,8 +7672,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5305425" y="6257925"/>
-          <a:ext cx="1181100" cy="419100"/>
+          <a:off x="4825365" y="6669405"/>
+          <a:ext cx="1043940" cy="441960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7836,8 +7836,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9658350" y="3295650"/>
-          <a:ext cx="5572760" cy="5687060"/>
+          <a:off x="8698230" y="3512820"/>
+          <a:ext cx="5024120" cy="6064250"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7875,8 +7875,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4353560" y="2009775"/>
-          <a:ext cx="6529070" cy="428625"/>
+          <a:off x="3947160" y="2135505"/>
+          <a:ext cx="5857875" cy="462915"/>
           <a:chOff x="1590" y="4095"/>
           <a:chExt cx="8101" cy="765"/>
         </a:xfrm>
@@ -8243,8 +8243,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9498965" y="201295"/>
-          <a:ext cx="10744835" cy="9287510"/>
+          <a:off x="8553450" y="212725"/>
+          <a:ext cx="9716135" cy="9904730"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8282,8 +8282,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2026920" y="6746875"/>
-          <a:ext cx="9401810" cy="946785"/>
+          <a:off x="1957070" y="7009765"/>
+          <a:ext cx="8341360" cy="1003935"/>
           <a:chOff x="205" y="5945"/>
           <a:chExt cx="11745" cy="1641"/>
         </a:xfrm>
@@ -8707,8 +8707,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5581015" y="3257550"/>
-          <a:ext cx="4799965" cy="3266440"/>
+          <a:off x="5024755" y="3474720"/>
+          <a:ext cx="4365625" cy="3300730"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8988,7 +8988,7 @@
       <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
@@ -9000,14 +9000,14 @@
   <sheetPr/>
   <dimension ref="D5:J16"/>
   <sheetViews>
-    <sheetView topLeftCell="K22" workbookViewId="0">
+    <sheetView topLeftCell="K13" workbookViewId="0">
       <selection activeCell="S65" sqref="S65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="4" max="4" width="12.875" customWidth="1"/>
-    <col min="10" max="10" width="30.2833333333333" customWidth="1"/>
+    <col min="4" max="4" width="12.8796296296296" customWidth="1"/>
+    <col min="10" max="10" width="30.287037037037" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="9:10">
@@ -9040,13 +9040,13 @@
   <sheetPr/>
   <dimension ref="C5:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14166666666667" defaultRowHeight="13.5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelCol="2"/>
   <cols>
-    <col min="3" max="3" width="22.425" customWidth="1"/>
+    <col min="3" max="3" width="22.4259259259259" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="3:3">
@@ -9085,14 +9085,14 @@
   <sheetPr/>
   <dimension ref="B3:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14166666666667" defaultRowHeight="13.5" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelCol="3"/>
   <cols>
-    <col min="2" max="2" width="32.425" customWidth="1"/>
-    <col min="3" max="3" width="31.425" customWidth="1"/>
+    <col min="2" max="2" width="32.4259259259259" customWidth="1"/>
+    <col min="3" max="3" width="31.4259259259259" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="23" customWidth="1"/>
@@ -9166,7 +9166,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="20" ht="175.5" spans="2:3">
+    <row r="20" ht="172.8" spans="2:3">
       <c r="B20" t="s">
         <v>256</v>
       </c>
@@ -9236,11 +9236,11 @@
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14166666666667" defaultRowHeight="13.5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelCol="7"/>
   <cols>
-    <col min="2" max="2" width="55.425" customWidth="1"/>
+    <col min="2" max="2" width="55.4259259259259" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="8" max="8" width="77.1416666666667" customWidth="1"/>
+    <col min="8" max="8" width="77.1388888888889" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" ht="15" spans="3:3">
@@ -9393,10 +9393,10 @@
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89166666666667" defaultRowHeight="13.5" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="4"/>
   <cols>
-    <col min="2" max="2" width="15.875" customWidth="1"/>
-    <col min="3" max="3" width="30.625" customWidth="1"/>
+    <col min="2" max="2" width="15.8796296296296" customWidth="1"/>
+    <col min="3" max="3" width="30.6296296296296" customWidth="1"/>
     <col min="4" max="4" width="74" customWidth="1"/>
     <col min="5" max="5" width="54" customWidth="1"/>
   </cols>
@@ -9544,7 +9544,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" ht="81" spans="2:5">
+    <row r="21" ht="86.4" spans="2:5">
       <c r="B21" s="29" t="s">
         <v>57</v>
       </c>
@@ -9674,7 +9674,7 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="6"/>
   <sheetData>
     <row r="2" spans="5:5">
       <c r="E2" s="3" t="s">
@@ -9845,17 +9845,17 @@
   <sheetPr/>
   <dimension ref="G10:N44"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E13" workbookViewId="0">
       <selection activeCell="M30" sqref="M30:N30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="7" max="7" width="14.75" customWidth="1"/>
     <col min="8" max="8" width="12.75" customWidth="1"/>
-    <col min="9" max="9" width="12.1333333333333" customWidth="1"/>
+    <col min="9" max="9" width="12.1296296296296" customWidth="1"/>
     <col min="10" max="10" width="13.25" customWidth="1"/>
-    <col min="11" max="11" width="13.3833333333333" customWidth="1"/>
+    <col min="11" max="11" width="13.3796296296296" customWidth="1"/>
     <col min="12" max="12" width="19" customWidth="1"/>
     <col min="13" max="13" width="13" customWidth="1"/>
     <col min="14" max="14" width="13.75" customWidth="1"/>
@@ -10276,11 +10276,11 @@
   <sheetPr/>
   <dimension ref="K9"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="9" spans="11:11">
       <c r="K9" s="3" t="s">
@@ -10302,11 +10302,11 @@
   <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
@@ -10319,11 +10319,11 @@
   <sheetPr/>
   <dimension ref="G50:G52"/>
   <sheetViews>
-    <sheetView topLeftCell="E22" workbookViewId="0">
+    <sheetView topLeftCell="E25" workbookViewId="0">
       <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="6"/>
   <sheetData>
     <row r="50" spans="7:7">
       <c r="G50" t="s">
@@ -10356,13 +10356,13 @@
       <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="12.875" customWidth="1"/>
-    <col min="4" max="4" width="13.5083333333333" customWidth="1"/>
-    <col min="7" max="7" width="17.2833333333333"/>
-    <col min="8" max="8" width="26.625" customWidth="1"/>
-    <col min="9" max="9" width="17.2833333333333"/>
+    <col min="2" max="2" width="12.8796296296296" customWidth="1"/>
+    <col min="4" max="4" width="13.5092592592593" customWidth="1"/>
+    <col min="7" max="7" width="17.287037037037"/>
+    <col min="8" max="8" width="26.6296296296296" customWidth="1"/>
+    <col min="9" max="9" width="17.287037037037"/>
   </cols>
   <sheetData>
     <row r="8" spans="2:10">

</xml_diff>